<commit_message>
Aula do dia 02/09/2025.
</commit_message>
<xml_diff>
--- a/banco_conexao/01_crud_uma_entidade/planilhas_exportadas/pessoas.xlsx
+++ b/banco_conexao/01_crud_uma_entidade/planilhas_exportadas/pessoas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -675,6 +675,46 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>13</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Milena Raquel Pereira</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>milenaraquelpereira@acquire.com.br</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>27/07/1965</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>14</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Sérgio Diego Da Rocha</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>sergiodiegodarocha@catsfeelings.com.br</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>06/01/2007</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>